<commit_message>
Added rpa_info and time_line func
</commit_message>
<xml_diff>
--- a/Katal.xlsx
+++ b/Katal.xlsx
@@ -686,8 +686,8 @@
   <dimension ref="A1:BF41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BF20" sqref="BF20"/>
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AI21" sqref="AI21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3493,6 +3493,26 @@
       </c>
       <c r="Z20">
         <v>4125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AC21">
+        <v>38</v>
+      </c>
+      <c r="AD21">
+        <v>55</v>
+      </c>
+      <c r="AE21">
+        <v>101</v>
+      </c>
+      <c r="AF21">
+        <v>150</v>
+      </c>
+      <c r="AG21">
+        <v>161</v>
+      </c>
+      <c r="AH21">
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started developing of GUI
</commit_message>
<xml_diff>
--- a/Katal.xlsx
+++ b/Katal.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
   <si>
     <t>Радиус АС</t>
   </si>
@@ -297,9 +297,6 @@
     <t>ПС-750-кс</t>
   </si>
   <si>
-    <t>AC 2х70/11</t>
-  </si>
-  <si>
     <t>ПБ(л)-330-4-1</t>
   </si>
   <si>
@@ -340,6 +337,12 @@
   </si>
   <si>
     <t>ЖД-Н</t>
+  </si>
+  <si>
+    <t>Шунт</t>
+  </si>
+  <si>
+    <t>Терм. стойкость, кА^2*c</t>
   </si>
 </sst>
 </file>
@@ -686,13 +689,13 @@
   <dimension ref="A1:BF41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AI21" sqref="AI21"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -835,10 +838,10 @@
         <v>43</v>
       </c>
       <c r="AH1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI1" t="s">
         <v>94</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>95</v>
       </c>
       <c r="AJ1" t="s">
         <v>44</v>
@@ -874,40 +877,40 @@
         <v>92</v>
       </c>
       <c r="AU1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AV1" t="s">
         <v>96</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>97</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>98</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>99</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>100</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>101</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>102</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>103</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>104</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>105</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>106</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
@@ -3180,7 +3183,7 @@
         <v>82</v>
       </c>
       <c r="AJ17" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="AK17" s="1"/>
       <c r="AL17" s="1"/>
@@ -3293,8 +3296,8 @@
       <c r="AI18" s="1">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="AJ18">
-        <v>4.7750000000000001E-2</v>
+      <c r="AJ18" s="1">
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="AK18" s="1"/>
       <c r="AL18" s="1"/>
@@ -3407,8 +3410,8 @@
       <c r="AI19" s="1">
         <v>1000000000000000</v>
       </c>
-      <c r="AJ19">
-        <v>0.21099999999999999</v>
+      <c r="AJ19" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AK19" s="1"/>
       <c r="AL19" s="1"/>
@@ -3496,6 +3499,9 @@
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
       <c r="AC21">
         <v>38</v>
       </c>

</xml_diff>